<commit_message>
Modify CI List with the new Files (App,BSW,Debug,MCAL)
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/CI_List/CI List.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/CI_List/CI List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>Project Name:</t>
   </si>
@@ -101,6 +101,75 @@
   </si>
   <si>
     <t>Test Result</t>
+  </si>
+  <si>
+    <t>CDD_LCD,CDD_DIO,CDD_TS,CDD_EEPROM,HLD</t>
+  </si>
+  <si>
+    <t>Test-Cases.docx</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>BSW</t>
+  </si>
+  <si>
+    <t>MCAL</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>App.c</t>
+  </si>
+  <si>
+    <t>Lcd</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>LCD_config.h,LCD_interface.h,LCD_private.h,LCD_prog.c</t>
+  </si>
+  <si>
+    <t>Shared liberary</t>
+  </si>
+  <si>
+    <t>Conc.h,delay_config.h,delay.h,Types.h,util.h</t>
+  </si>
+  <si>
+    <t>TACTILE_config.h,TACTILE_interface.h,TACTILE_private.h,TACTILE_prog.c</t>
+  </si>
+  <si>
+    <t>DIO</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>DIO_config.h,DIO_interface.h,DIO_private.h,DIO_prog.c</t>
+  </si>
+  <si>
+    <t>EEPROM_config.h,EEPROM_interface.h,EEPROM_private.h,EEPROM_prog.c</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>LCD_Prog.d,LCD_Prog.o</t>
+  </si>
+  <si>
+    <t>TACTILE_Prog.d,TACTILE_Prog.o</t>
+  </si>
+  <si>
+    <t>DIO_Prog.d,DIO_Prog.o</t>
+  </si>
+  <si>
+    <t>EEPROM_Prog.d,EEPROM_Prog.o</t>
+  </si>
+  <si>
+    <t>App.d,App.o</t>
   </si>
 </sst>
 </file>
@@ -122,6 +191,7 @@
       <b/>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -131,6 +201,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -153,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -293,11 +364,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -311,6 +444,48 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -328,15 +503,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -630,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G18"/>
+  <dimension ref="B1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="I25" sqref="I25:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,179 +808,468 @@
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="8" max="10" width="8.5546875" customWidth="1"/>
+    <col min="11" max="11" width="38" customWidth="1"/>
+    <col min="12" max="12" width="67.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="28"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="15"/>
-      <c r="C7" s="13" t="s">
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="26"/>
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="15"/>
-      <c r="C8" s="13" t="s">
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="26"/>
+      <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-      <c r="C9" s="13" t="s">
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="26"/>
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="15"/>
-      <c r="C10" s="13" t="s">
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="26"/>
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
-      <c r="C11" s="13" t="s">
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="26"/>
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="15"/>
-      <c r="C12" s="13" t="s">
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="26"/>
+      <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="16"/>
-      <c r="C13" s="13" t="s">
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="27"/>
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16"/>
-      <c r="C15" s="13" t="s">
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="26"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="26"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="26"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="26"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="26"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="26"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="26"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="26"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="K22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22" s="7"/>
+    </row>
+    <row r="23" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="26"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="7"/>
+    </row>
+    <row r="24" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="26"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="2:14" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="26"/>
+      <c r="C25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="27"/>
+      <c r="C26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="2:14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:14" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="95">
+    <mergeCell ref="G22:H23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="B14:B26"/>
+    <mergeCell ref="C14:D24"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E15:F17"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="E20:F24"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C5:D5"/>
@@ -827,6 +1282,65 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H21"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add files (App_config.h , App_private.h)
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/CI_List/CI List.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/CI_List/CI List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16668" windowHeight="7728"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12636" windowHeight="6036"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>Debug</t>
   </si>
   <si>
-    <t>App.c</t>
-  </si>
-  <si>
     <t>Lcd</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>App.d,App.o</t>
+  </si>
+  <si>
+    <t>App.c,App_config.h,App_private.h</t>
   </si>
 </sst>
 </file>
@@ -444,77 +444,77 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25:J25"/>
+    <sheetView tabSelected="1" topLeftCell="J12" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,24 +818,24 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -845,399 +845,399 @@
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10" t="s">
+      <c r="H5" s="27"/>
+      <c r="I5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="18" t="s">
+      <c r="J5" s="27"/>
+      <c r="K5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="11"/>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="26"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="26"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="5" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="18"/>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="26"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="26"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="26"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="26"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="27"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="6" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="6" t="s">
+      <c r="F14" s="12"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="14"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="26"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="12" t="s">
+      <c r="H15" s="12"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="14"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="12"/>
+    </row>
+    <row r="17" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="14"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="12"/>
+    </row>
+    <row r="18" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="14"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" s="12"/>
+    </row>
+    <row r="19" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="14"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="12"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="14"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="6" t="s">
+      <c r="H20" s="17"/>
+      <c r="I20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="14"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="26"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="26"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="6" t="s">
+      <c r="J21" s="10"/>
+      <c r="K21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21" s="12"/>
+    </row>
+    <row r="22" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="14"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="26"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="8" t="s">
+      <c r="J22" s="10"/>
+      <c r="K22" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="12"/>
+    </row>
+    <row r="23" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="14"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="26"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="26"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="26"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="26"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="6" t="s">
+      <c r="J23" s="12"/>
+      <c r="K23" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="7"/>
-    </row>
-    <row r="23" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="26"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="6" t="s">
+      <c r="L23" s="12"/>
+    </row>
+    <row r="24" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="14"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="26"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="18"/>
     </row>
     <row r="25" spans="2:14" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="26"/>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5" t="s">
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="L25" s="5"/>
+      <c r="L25" s="18"/>
     </row>
     <row r="26" spans="2:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="27"/>
-      <c r="C26" s="5" t="s">
+      <c r="B26" s="15"/>
+      <c r="C26" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5" t="s">
+      <c r="D26" s="18"/>
+      <c r="E26" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5" t="s">
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L26" s="5"/>
+      <c r="L26" s="18"/>
     </row>
     <row r="27" spans="2:14" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:14" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1246,29 +1246,61 @@
     <row r="31" spans="2:14" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="G22:H23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="B14:B26"/>
-    <mergeCell ref="C14:D24"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F17"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="E20:F24"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H21"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:F3"/>
@@ -1285,62 +1317,30 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B14:B26"/>
+    <mergeCell ref="C14:D24"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F17"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="E20:F24"/>
+    <mergeCell ref="G22:H23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
     <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H21"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>